<commit_message>
Added content descriptions to some things so that I get less annoying warnings in the prelaunch report
</commit_message>
<xml_diff>
--- a/Feature_Tracker.xlsx
+++ b/Feature_Tracker.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E488314-0852-4CC4-A8E5-869C7502AAC9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A76100E-7A4C-4446-8D86-0065648F7C47}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>Feature</t>
   </si>
@@ -56,6 +56,27 @@
   </si>
   <si>
     <t>_dharwin - Reddit /r/dnd</t>
+  </si>
+  <si>
+    <t>Nitrogen06 - Reddit /r/rpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fate Dice </t>
+  </si>
+  <si>
+    <t>Have a custom type of dice that rolls between -1 and 1</t>
+  </si>
+  <si>
+    <t>1.4.1</t>
+  </si>
+  <si>
+    <t>1.3.0</t>
+  </si>
+  <si>
+    <t>joethomp - Reddit /r/rpg</t>
+  </si>
+  <si>
+    <t>UraniumKnight - Reddit /r/rpg</t>
   </si>
 </sst>
 </file>
@@ -373,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -385,10 +406,11 @@
     <col min="2" max="2" width="104.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="34.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -402,18 +424,27 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
       <c r="D2" t="s">
         <v>11</v>
       </c>
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -424,7 +455,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -433,6 +464,20 @@
       </c>
       <c r="D4" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the install tracker and feature tracker
Updated the die and roller classes to be separate as they really are not the same thing

Reworked how rolls are done so that I can do advantage/disadvantage and drop high/low stuff
</commit_message>
<xml_diff>
--- a/Feature_Tracker.xlsx
+++ b/Feature_Tracker.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A76100E-7A4C-4446-8D86-0065648F7C47}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{187E496F-36F9-46F0-B50D-CB64EA6AAD7F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
     <t>Feature</t>
   </si>
@@ -77,6 +77,36 @@
   </si>
   <si>
     <t>UraniumKnight - Reddit /r/rpg</t>
+  </si>
+  <si>
+    <t>Have per die modifiers</t>
+  </si>
+  <si>
+    <t>Instead of having a single modifier that is on a per roll basis, have it on a per die basis</t>
+  </si>
+  <si>
+    <t>When you have many different saved rolls it can be overwhelming, groups of rolls would be nice</t>
+  </si>
+  <si>
+    <t>Add Color</t>
+  </si>
+  <si>
+    <t>Having all the dice be in gray scale is not fun to look at</t>
+  </si>
+  <si>
+    <t>Kris Fiala</t>
+  </si>
+  <si>
+    <t>Roll groupings</t>
+  </si>
+  <si>
+    <t>Roll Variants</t>
+  </si>
+  <si>
+    <t>Allow for setting variant versions of a roll, i.e. d6 vs d6(poison) vs d6(green)</t>
+  </si>
+  <si>
+    <t>Weston Fiala</t>
   </si>
 </sst>
 </file>
@@ -394,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -410,7 +440,7 @@
     <col min="6" max="6" width="24.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -424,7 +454,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -438,46 +468,90 @@
         <v>11</v>
       </c>
       <c r="E2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" t="s">
         <v>18</v>
       </c>
-      <c r="F2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" t="s">
-        <v>17</v>
+      <c r="E7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed up the bottom bar for the simple roller so that it is easier to maintain.
</commit_message>
<xml_diff>
--- a/Feature_Tracker.xlsx
+++ b/Feature_Tracker.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{187E496F-36F9-46F0-B50D-CB64EA6AAD7F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CFB6EDD-1F28-4647-9127-F91ECD5F0BFD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -427,7 +427,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated the feature tracker with a new request
</commit_message>
<xml_diff>
--- a/Feature_Tracker.xlsx
+++ b/Feature_Tracker.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CFB6EDD-1F28-4647-9127-F91ECD5F0BFD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46981174-3464-42E5-9FB9-21C8137CC16F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
   <si>
     <t>Feature</t>
   </si>
@@ -107,6 +107,21 @@
   </si>
   <si>
     <t>Weston Fiala</t>
+  </si>
+  <si>
+    <t>User Profiles</t>
+  </si>
+  <si>
+    <t>BlankTheorist - Reddit /r/dnd</t>
+  </si>
+  <si>
+    <t>Allow for saving custom rolls into a user profile so that they do not bleed into other rolls</t>
+  </si>
+  <si>
+    <t>Roll Negative Die</t>
+  </si>
+  <si>
+    <t>In order to roll with Bane, I need to roll a negative d4. Right now you can only roll positively</t>
   </si>
 </sst>
 </file>
@@ -424,10 +439,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -503,6 +518,12 @@
       <c r="B5" t="s">
         <v>21</v>
       </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -551,6 +572,28 @@
         <v>27</v>
       </c>
       <c r="D9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added animations and sub fabs to the create a die fab button
Removes one of the die creation dialogs. Trying to get away from dialogs when possible.
</commit_message>
<xml_diff>
--- a/Feature_Tracker.xlsx
+++ b/Feature_Tracker.xlsx
@@ -3,13 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46981174-3464-42E5-9FB9-21C8137CC16F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52F63356-897E-421B-814D-899D26EC02A9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$12</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -20,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="39">
   <si>
     <t>Feature</t>
   </si>
@@ -122,6 +125,21 @@
   </si>
   <si>
     <t>In order to roll with Bane, I need to roll a negative d4. Right now you can only roll positively</t>
+  </si>
+  <si>
+    <t>1.5.0</t>
+  </si>
+  <si>
+    <t>Restore history button</t>
+  </si>
+  <si>
+    <t>Removing all the history on accident can be a pain. Is it possible to restore that with a button somewhere?</t>
+  </si>
+  <si>
+    <t>1.5.1</t>
+  </si>
+  <si>
+    <t>Bart van den Hoek - Store Review</t>
   </si>
 </sst>
 </file>
@@ -439,10 +457,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E11"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -469,7 +488,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -486,7 +505,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -500,12 +519,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
       <c r="B4" t="s">
         <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>34</v>
       </c>
       <c r="D4" t="s">
         <v>12</v>
@@ -525,13 +547,16 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
       </c>
+      <c r="C6" t="s">
+        <v>34</v>
+      </c>
       <c r="D6" t="s">
         <v>7</v>
       </c>
@@ -539,12 +564,15 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>34</v>
       </c>
       <c r="D7" t="s">
         <v>7</v>
@@ -597,7 +625,26 @@
         <v>28</v>
       </c>
     </row>
+    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:E12" xr:uid="{B4F77D32-E558-4F22-95C5-F86840C342A2}">
+    <filterColumn colId="2">
+      <filters blank="1"/>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated install tracker and the feature tracker
</commit_message>
<xml_diff>
--- a/Feature_Tracker.xlsx
+++ b/Feature_Tracker.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52F63356-897E-421B-814D-899D26EC02A9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC6174F4-BFC1-4914-8B4A-292DBDE5EF34}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -13,17 +13,22 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$12</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="42">
   <si>
     <t>Feature</t>
   </si>
@@ -140,6 +145,15 @@
   </si>
   <si>
     <t>Bart van den Hoek - Store Review</t>
+  </si>
+  <si>
+    <t>Reroll below threshold</t>
+  </si>
+  <si>
+    <t>Re-roll dice that are below a certain threshold, like 1 &amp; 2 for great weapon master</t>
+  </si>
+  <si>
+    <t>Sean Steele - ssteele1812@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -457,11 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -488,7 +501,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -505,7 +518,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -519,7 +532,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -547,7 +560,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -564,7 +577,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -625,7 +638,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>35</v>
       </c>
@@ -639,12 +652,19 @@
         <v>38</v>
       </c>
     </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" t="s">
+        <v>41</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:E12" xr:uid="{B4F77D32-E558-4F22-95C5-F86840C342A2}">
-    <filterColumn colId="2">
-      <filters blank="1"/>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:E12" xr:uid="{B4F77D32-E558-4F22-95C5-F86840C342A2}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated the install tracker
</commit_message>
<xml_diff>
--- a/Feature_Tracker.xlsx
+++ b/Feature_Tracker.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC6174F4-BFC1-4914-8B4A-292DBDE5EF34}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA925CCC-F52A-4755-AA88-3AB6CB64A4C7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,7 +11,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$12</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$13</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="43">
   <si>
     <t>Feature</t>
   </si>
@@ -154,6 +154,9 @@
   </si>
   <si>
     <t>Sean Steele - ssteele1812@gmail.com</t>
+  </si>
+  <si>
+    <t>1.5.3</t>
   </si>
 </sst>
 </file>
@@ -471,10 +474,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -501,7 +505,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -518,7 +522,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -532,7 +536,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -560,7 +564,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -577,7 +581,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -627,18 +631,21 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>32</v>
       </c>
       <c r="B11" t="s">
         <v>33</v>
       </c>
+      <c r="C11" t="s">
+        <v>42</v>
+      </c>
       <c r="D11" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>35</v>
       </c>
@@ -664,7 +671,11 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E12" xr:uid="{B4F77D32-E558-4F22-95C5-F86840C342A2}"/>
+  <autoFilter ref="A1:E13" xr:uid="{B4F77D32-E558-4F22-95C5-F86840C342A2}">
+    <filterColumn colId="2">
+      <filters blank="1"/>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Reworked how roll properties are added. New way makes it much easier to add new types of roll properties, like reroll under X value.
</commit_message>
<xml_diff>
--- a/Feature_Tracker.xlsx
+++ b/Feature_Tracker.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA925CCC-F52A-4755-AA88-3AB6CB64A4C7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D79F460C-2680-4371-B812-69FCDA510979}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="46">
   <si>
     <t>Feature</t>
   </si>
@@ -157,6 +157,15 @@
   </si>
   <si>
     <t>1.5.3</t>
+  </si>
+  <si>
+    <t>Exploding dice</t>
+  </si>
+  <si>
+    <t>When you roll maximum on a die, keep rolling until you don't</t>
+  </si>
+  <si>
+    <t>Mike Combs - Store review</t>
   </si>
 </sst>
 </file>
@@ -475,10 +484,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -670,6 +679,17 @@
         <v>41</v>
       </c>
     </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" t="s">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:E13" xr:uid="{B4F77D32-E558-4F22-95C5-F86840C342A2}">
     <filterColumn colId="2">

</xml_diff>

<commit_message>
Added all the new types of properties to the rolls and made them work! hopefully everything works out when I post it!
</commit_message>
<xml_diff>
--- a/Feature_Tracker.xlsx
+++ b/Feature_Tracker.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D79F460C-2680-4371-B812-69FCDA510979}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{468C34F0-3E61-48A0-8B7E-976966E67591}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="48">
   <si>
     <t>Feature</t>
   </si>
@@ -166,6 +166,12 @@
   </si>
   <si>
     <t>Mike Combs - Store review</t>
+  </si>
+  <si>
+    <t>Minimum roll value</t>
+  </si>
+  <si>
+    <t>When you roll below a threshold, treat any roll that is less than that threshold as that threshold.</t>
   </si>
 </sst>
 </file>
@@ -484,10 +490,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -690,6 +696,17 @@
         <v>45</v>
       </c>
     </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:E13" xr:uid="{B4F77D32-E558-4F22-95C5-F86840C342A2}">
     <filterColumn colId="2">

</xml_diff>

<commit_message>
Updated the feature tracker with the things that are now finished.
</commit_message>
<xml_diff>
--- a/Feature_Tracker.xlsx
+++ b/Feature_Tracker.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{468C34F0-3E61-48A0-8B7E-976966E67591}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3184B524-9F0E-4A5E-9679-39F1D4AE1018}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,7 +11,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$13</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$18</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="56">
   <si>
     <t>Feature</t>
   </si>
@@ -172,6 +172,30 @@
   </si>
   <si>
     <t>When you roll below a threshold, treat any roll that is less than that threshold as that threshold.</t>
+  </si>
+  <si>
+    <t>Horizontal custom rolls</t>
+  </si>
+  <si>
+    <t>Having a bunch of the same icon with little text is not an efficient use of space. Convert to horizontal and remove icon.</t>
+  </si>
+  <si>
+    <t>1.5.6</t>
+  </si>
+  <si>
+    <t>Add Genesys dice</t>
+  </si>
+  <si>
+    <t>The game Genesys uses dice. Add them in.</t>
+  </si>
+  <si>
+    <t>Add Fantasy Flight Star Wars dice</t>
+  </si>
+  <si>
+    <t>The game Fantasy Flight Star Wars uses dice. Add them in.</t>
+  </si>
+  <si>
+    <t>Joseph Thompson - Store Review</t>
   </si>
 </sst>
 </file>
@@ -490,10 +514,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -674,41 +698,83 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>39</v>
       </c>
       <c r="B13" t="s">
         <v>40</v>
       </c>
+      <c r="C13" t="s">
+        <v>50</v>
+      </c>
       <c r="D13" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>43</v>
       </c>
       <c r="B14" t="s">
         <v>44</v>
       </c>
+      <c r="C14" t="s">
+        <v>50</v>
+      </c>
       <c r="D14" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>46</v>
       </c>
       <c r="B15" t="s">
         <v>47</v>
       </c>
+      <c r="C15" t="s">
+        <v>50</v>
+      </c>
       <c r="D15" t="s">
         <v>28</v>
       </c>
     </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" t="s">
+        <v>52</v>
+      </c>
+      <c r="D17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" t="s">
+        <v>55</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:E13" xr:uid="{B4F77D32-E558-4F22-95C5-F86840C342A2}">
+  <autoFilter ref="A1:E18" xr:uid="{B4F77D32-E558-4F22-95C5-F86840C342A2}">
     <filterColumn colId="2">
       <filters blank="1"/>
     </filterColumn>

</xml_diff>

<commit_message>
Really fast rework of the saved roller tab. Already looks better with all of the details being shown at once.
</commit_message>
<xml_diff>
--- a/Feature_Tracker.xlsx
+++ b/Feature_Tracker.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3184B524-9F0E-4A5E-9679-39F1D4AE1018}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7530110D-6D1C-49EE-85BD-CAA95DF81BBA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="56">
   <si>
     <t>Feature</t>
   </si>
@@ -517,7 +517,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -750,6 +750,9 @@
       <c r="D16" t="s">
         <v>28</v>
       </c>
+      <c r="E16" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">

</xml_diff>

<commit_message>
Updated the install tracker to account for the new horizontal layout in saved rolls
</commit_message>
<xml_diff>
--- a/Feature_Tracker.xlsx
+++ b/Feature_Tracker.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7530110D-6D1C-49EE-85BD-CAA95DF81BBA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47740ABE-D7FF-4C89-AA4C-CD7255D64FDD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="59">
   <si>
     <t>Feature</t>
   </si>
@@ -196,6 +196,15 @@
   </si>
   <si>
     <t>Joseph Thompson - Store Review</t>
+  </si>
+  <si>
+    <t>1.5.7</t>
+  </si>
+  <si>
+    <t>Edit Saved Rolls</t>
+  </si>
+  <si>
+    <t>Allow the user to edit saved rolls easily. Auto move to custom roll tab, and fill out all the die in the roll.</t>
   </si>
 </sst>
 </file>
@@ -514,10 +523,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -747,11 +756,11 @@
       <c r="B16" t="s">
         <v>49</v>
       </c>
+      <c r="C16" t="s">
+        <v>56</v>
+      </c>
       <c r="D16" t="s">
         <v>28</v>
-      </c>
-      <c r="E16" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -774,6 +783,17 @@
       </c>
       <c r="D18" t="s">
         <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>57</v>
+      </c>
+      <c r="B19" t="s">
+        <v>58</v>
+      </c>
+      <c r="D19" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added critical hit and critical miss sound effects. Triple air horn, and wilhelm scream.
Fixed a bug where drop high/low was broken.
</commit_message>
<xml_diff>
--- a/Feature_Tracker.xlsx
+++ b/Feature_Tracker.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47740ABE-D7FF-4C89-AA4C-CD7255D64FDD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18530CBE-4673-4485-BB61-8C85D89F5777}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,7 +11,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$18</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$20</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="64">
   <si>
     <t>Feature</t>
   </si>
@@ -205,6 +205,21 @@
   </si>
   <si>
     <t>Allow the user to edit saved rolls easily. Auto move to custom roll tab, and fill out all the die in the roll.</t>
+  </si>
+  <si>
+    <t>Crit and Crit Fail Sounds</t>
+  </si>
+  <si>
+    <t>When you roll minimum or maximum on a roll, do the willhelm scream or the air horn in order</t>
+  </si>
+  <si>
+    <t>Stefan Titus</t>
+  </si>
+  <si>
+    <t>Roll Again Button</t>
+  </si>
+  <si>
+    <t>Stop the dismissing by random click for the results, make it so you have a roll again, and close buttons.</t>
   </si>
 </sst>
 </file>
@@ -523,10 +538,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -749,7 +764,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>48</v>
       </c>
@@ -796,8 +811,30 @@
         <v>41</v>
       </c>
     </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20" t="s">
+        <v>60</v>
+      </c>
+      <c r="D20" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" t="s">
+        <v>63</v>
+      </c>
+      <c r="D21" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:E18" xr:uid="{B4F77D32-E558-4F22-95C5-F86840C342A2}">
+  <autoFilter ref="A1:E20" xr:uid="{B4F77D32-E558-4F22-95C5-F86840C342A2}">
     <filterColumn colId="2">
       <filters blank="1"/>
     </filterColumn>

</xml_diff>

<commit_message>
Generated the 1.5.8 bundle and bumped version to 1.5.9
</commit_message>
<xml_diff>
--- a/Feature_Tracker.xlsx
+++ b/Feature_Tracker.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18530CBE-4673-4485-BB61-8C85D89F5777}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{404ED864-B171-4285-A51A-C4A249C1A5F6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,7 +11,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$20</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$21</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="65">
   <si>
     <t>Feature</t>
   </si>
@@ -210,9 +210,6 @@
     <t>Crit and Crit Fail Sounds</t>
   </si>
   <si>
-    <t>When you roll minimum or maximum on a roll, do the willhelm scream or the air horn in order</t>
-  </si>
-  <si>
     <t>Stefan Titus</t>
   </si>
   <si>
@@ -220,6 +217,12 @@
   </si>
   <si>
     <t>Stop the dismissing by random click for the results, make it so you have a roll again, and close buttons.</t>
+  </si>
+  <si>
+    <t>1.5.8</t>
+  </si>
+  <si>
+    <t>When you roll minimum or maximum on a roll, do the willhelm scream or the air horn sound effects</t>
   </si>
 </sst>
 </file>
@@ -541,7 +544,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -811,30 +814,33 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>59</v>
       </c>
       <c r="B20" t="s">
+        <v>64</v>
+      </c>
+      <c r="C20" t="s">
+        <v>63</v>
+      </c>
+      <c r="D20" t="s">
         <v>60</v>
-      </c>
-      <c r="D20" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" t="s">
         <v>62</v>
-      </c>
-      <c r="B21" t="s">
-        <v>63</v>
       </c>
       <c r="D21" t="s">
         <v>28</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E20" xr:uid="{B4F77D32-E558-4F22-95C5-F86840C342A2}">
+  <autoFilter ref="A1:E21" xr:uid="{B4F77D32-E558-4F22-95C5-F86840C342A2}">
     <filterColumn colId="2">
       <filters blank="1"/>
     </filterColumn>

</xml_diff>

<commit_message>
Updated the feature tracker and install tracker
</commit_message>
<xml_diff>
--- a/Feature_Tracker.xlsx
+++ b/Feature_Tracker.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{404ED864-B171-4285-A51A-C4A249C1A5F6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72459399-8E18-41E2-A7F3-CC42134B97AB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="66">
   <si>
     <t>Feature</t>
   </si>
@@ -223,6 +223,9 @@
   </si>
   <si>
     <t>When you roll minimum or maximum on a roll, do the willhelm scream or the air horn sound effects</t>
+  </si>
+  <si>
+    <t>Edward Robbins - Store Review</t>
   </si>
 </sst>
 </file>
@@ -781,7 +784,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>51</v>
       </c>
@@ -792,7 +795,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>53</v>
       </c>
@@ -803,7 +806,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>57</v>
       </c>
@@ -813,8 +816,11 @@
       <c r="D19" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>59</v>
       </c>
@@ -828,7 +834,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>61</v>
       </c>

</xml_diff>

<commit_message>
Updated install tracker and feature tracker
</commit_message>
<xml_diff>
--- a/Feature_Tracker.xlsx
+++ b/Feature_Tracker.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72459399-8E18-41E2-A7F3-CC42134B97AB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8CC082B-8519-4983-B0A9-538B6F244DD4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="69">
   <si>
     <t>Feature</t>
   </si>
@@ -226,6 +226,15 @@
   </si>
   <si>
     <t>Edward Robbins - Store Review</t>
+  </si>
+  <si>
+    <t>Set faces on a die</t>
+  </si>
+  <si>
+    <t>I want to be able to create imbalanced dice, ie 1,1,1,2,2,3</t>
+  </si>
+  <si>
+    <t>Alpha PiPi - Store Review</t>
   </si>
 </sst>
 </file>
@@ -544,10 +553,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -845,6 +854,17 @@
         <v>28</v>
       </c>
     </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>66</v>
+      </c>
+      <c r="B22" t="s">
+        <v>67</v>
+      </c>
+      <c r="D22" t="s">
+        <v>68</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:E21" xr:uid="{B4F77D32-E558-4F22-95C5-F86840C342A2}">
     <filterColumn colId="2">

</xml_diff>

<commit_message>
Added a new type of die, the ImbalancedDie. It allows you to add the faces that you want directly to a die.
Example ImbalancedDie - 1,1,1,2,2,3
</commit_message>
<xml_diff>
--- a/Feature_Tracker.xlsx
+++ b/Feature_Tracker.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8CC082B-8519-4983-B0A9-538B6F244DD4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB3C0161-3748-48AD-8242-DF3157169C48}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="69">
   <si>
     <t>Feature</t>
   </si>
@@ -556,7 +556,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -697,6 +697,9 @@
       <c r="D9" t="s">
         <v>28</v>
       </c>
+      <c r="E9" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">

</xml_diff>

<commit_message>
Updated the feature tracker.
</commit_message>
<xml_diff>
--- a/Feature_Tracker.xlsx
+++ b/Feature_Tracker.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6CBB8D9-8825-441F-B5D4-89F7F01B6383}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE285D82-811E-4F83-BEBB-51F1BC7C1773}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,7 +11,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$22</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$23</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="73">
   <si>
     <t>Feature</t>
   </si>
@@ -238,6 +238,15 @@
   </si>
   <si>
     <t>1.6.0</t>
+  </si>
+  <si>
+    <t>Edit Dice</t>
+  </si>
+  <si>
+    <t>I misnamed one of my custom dice and just want to tweek the name.</t>
+  </si>
+  <si>
+    <t>1.6.1</t>
   </si>
 </sst>
 </file>
@@ -556,10 +565,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -874,8 +883,22 @@
         <v>68</v>
       </c>
     </row>
+    <row r="23" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>70</v>
+      </c>
+      <c r="B23" t="s">
+        <v>71</v>
+      </c>
+      <c r="C23" t="s">
+        <v>72</v>
+      </c>
+      <c r="D23" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:E22" xr:uid="{B4F77D32-E558-4F22-95C5-F86840C342A2}">
+  <autoFilter ref="A1:E23" xr:uid="{B4F77D32-E558-4F22-95C5-F86840C342A2}">
     <filterColumn colId="2">
       <filters blank="1"/>
     </filterColumn>

</xml_diff>

<commit_message>
Generated the 1.6.2 bundle and bumped version to 1.6.3
</commit_message>
<xml_diff>
--- a/Feature_Tracker.xlsx
+++ b/Feature_Tracker.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE285D82-811E-4F83-BEBB-51F1BC7C1773}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC79D98C-CFF1-43AB-8579-8CE157ED3690}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="76">
   <si>
     <t>Feature</t>
   </si>
@@ -247,6 +247,15 @@
   </si>
   <si>
     <t>1.6.1</t>
+  </si>
+  <si>
+    <t>1.6.2</t>
+  </si>
+  <si>
+    <t>Add multiples of dice to roll</t>
+  </si>
+  <si>
+    <t>I want to roll 6 d20s each with their own modifier in one roll</t>
   </si>
 </sst>
 </file>
@@ -565,10 +574,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -709,9 +718,6 @@
       <c r="D9" t="s">
         <v>28</v>
       </c>
-      <c r="E9" t="s">
-        <v>65</v>
-      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -837,6 +843,9 @@
       <c r="B19" t="s">
         <v>58</v>
       </c>
+      <c r="C19" t="s">
+        <v>73</v>
+      </c>
       <c r="D19" t="s">
         <v>41</v>
       </c>
@@ -895,6 +904,17 @@
       </c>
       <c r="D23" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>74</v>
+      </c>
+      <c r="B24" t="s">
+        <v>75</v>
+      </c>
+      <c r="D24" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated install and Feature trackers
</commit_message>
<xml_diff>
--- a/Feature_Tracker.xlsx
+++ b/Feature_Tracker.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC79D98C-CFF1-43AB-8579-8CE157ED3690}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7F0CDBA-6A65-41E0-9CA7-C6D48C18C410}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,7 +11,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$23</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$24</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="76">
   <si>
     <t>Feature</t>
   </si>
@@ -574,10 +574,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -590,7 +590,7 @@
     <col min="6" max="6" width="24.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -604,7 +604,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -621,7 +621,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -635,7 +635,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -649,7 +649,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -662,8 +662,11 @@
       <c r="E5" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -680,7 +683,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -697,7 +700,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -708,7 +711,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -719,7 +722,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -730,7 +733,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>32</v>
       </c>
@@ -744,7 +747,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>35</v>
       </c>
@@ -758,7 +761,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>39</v>
       </c>
@@ -772,7 +775,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>43</v>
       </c>
@@ -786,7 +789,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>46</v>
       </c>
@@ -800,7 +803,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>48</v>
       </c>
@@ -836,7 +839,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>57</v>
       </c>
@@ -918,7 +921,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E23" xr:uid="{B4F77D32-E558-4F22-95C5-F86840C342A2}">
+  <autoFilter ref="A1:E24" xr:uid="{B4F77D32-E558-4F22-95C5-F86840C342A2}">
     <filterColumn colId="2">
       <filters blank="1"/>
     </filterColumn>

</xml_diff>

<commit_message>
Made duration of roller based on time and not number of frames
</commit_message>
<xml_diff>
--- a/Feature_Tracker.xlsx
+++ b/Feature_Tracker.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7F0CDBA-6A65-41E0-9CA7-C6D48C18C410}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8E93367-2075-454B-8BAC-18A0FE401197}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="81">
   <si>
     <t>Feature</t>
   </si>
@@ -256,6 +256,21 @@
   </si>
   <si>
     <t>I want to roll 6 d20s each with their own modifier in one roll</t>
+  </si>
+  <si>
+    <t>Make roll time based</t>
+  </si>
+  <si>
+    <t>Rolls currently are based on a number of frames, not time. Switch to time.</t>
+  </si>
+  <si>
+    <t>Make average more accurate</t>
+  </si>
+  <si>
+    <t>The roll average only looks at the number of dice in a roll, and has nothing to do with all the roll properties</t>
+  </si>
+  <si>
+    <t>1.6.7</t>
   </si>
 </sst>
 </file>
@@ -574,10 +589,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -920,6 +935,31 @@
         <v>65</v>
       </c>
     </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>76</v>
+      </c>
+      <c r="B25" t="s">
+        <v>77</v>
+      </c>
+      <c r="C25" t="s">
+        <v>80</v>
+      </c>
+      <c r="D25" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>78</v>
+      </c>
+      <c r="B26" t="s">
+        <v>79</v>
+      </c>
+      <c r="D26" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:E24" xr:uid="{B4F77D32-E558-4F22-95C5-F86840C342A2}">
     <filterColumn colId="2">

</xml_diff>

<commit_message>
Added a roll again button to the roll results dialog
Changed the name of "average roll" to "expected result"
</commit_message>
<xml_diff>
--- a/Feature_Tracker.xlsx
+++ b/Feature_Tracker.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8E93367-2075-454B-8BAC-18A0FE401197}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10CC09C1-6F54-4E72-B993-15D591419396}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="81">
   <si>
     <t>Feature</t>
   </si>
@@ -592,7 +592,7 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -892,6 +892,9 @@
       <c r="B21" t="s">
         <v>62</v>
       </c>
+      <c r="C21" t="s">
+        <v>80</v>
+      </c>
       <c r="D21" t="s">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
Added a new field to saved rolls, categories. All rolls now have a category and a name. You can expand and collapse categories.
Changed the subtitle at top of screen when you move between tabs.
</commit_message>
<xml_diff>
--- a/Feature_Tracker.xlsx
+++ b/Feature_Tracker.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10CC09C1-6F54-4E72-B993-15D591419396}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F91BF3FB-FA2F-49E6-A9FE-B079D001634C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,7 +11,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$24</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$26</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -592,7 +592,7 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -885,7 +885,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>61</v>
       </c>
@@ -938,7 +938,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>76</v>
       </c>
@@ -964,7 +964,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E24" xr:uid="{B4F77D32-E558-4F22-95C5-F86840C342A2}">
+  <autoFilter ref="A1:E26" xr:uid="{B4F77D32-E558-4F22-95C5-F86840C342A2}">
     <filterColumn colId="2">
       <filters blank="1"/>
     </filterColumn>

</xml_diff>

<commit_message>
Tiny change to remove override prompt when editing a saved roll
Updated the feature tracker
</commit_message>
<xml_diff>
--- a/Feature_Tracker.xlsx
+++ b/Feature_Tracker.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F91BF3FB-FA2F-49E6-A9FE-B079D001634C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0E95EEB-F3F4-4A9B-93C3-493A91DAE5C5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="82">
   <si>
     <t>Feature</t>
   </si>
@@ -271,6 +271,9 @@
   </si>
   <si>
     <t>1.6.7</t>
+  </si>
+  <si>
+    <t>1.7.0</t>
   </si>
 </sst>
 </file>
@@ -592,7 +595,7 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -671,6 +674,9 @@
       <c r="B5" t="s">
         <v>21</v>
       </c>
+      <c r="C5" t="s">
+        <v>81</v>
+      </c>
       <c r="D5" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
Updated feature tracker and install tracker
</commit_message>
<xml_diff>
--- a/Feature_Tracker.xlsx
+++ b/Feature_Tracker.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03B73FCC-3C27-49AA-902E-2884611249B2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8565F34-874A-4F9C-A0D6-D920AE1D3210}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,7 +11,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$26</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$29</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="90">
   <si>
     <t>Feature</t>
   </si>
@@ -295,6 +295,9 @@
   </si>
   <si>
     <t>Never</t>
+  </si>
+  <si>
+    <t>1.7.2</t>
   </si>
 </sst>
 </file>
@@ -616,7 +619,7 @@
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -688,7 +691,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -859,7 +862,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>51</v>
       </c>
@@ -873,7 +876,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>53</v>
       </c>
@@ -996,23 +999,29 @@
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>82</v>
       </c>
       <c r="B27" t="s">
         <v>83</v>
       </c>
+      <c r="C27" t="s">
+        <v>89</v>
+      </c>
       <c r="D27" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>84</v>
       </c>
       <c r="B28" t="s">
         <v>87</v>
+      </c>
+      <c r="C28" t="s">
+        <v>89</v>
       </c>
       <c r="D28" t="s">
         <v>28</v>
@@ -1030,7 +1039,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E26" xr:uid="{B4F77D32-E558-4F22-95C5-F86840C342A2}">
+  <autoFilter ref="A1:E29" xr:uid="{B4F77D32-E558-4F22-95C5-F86840C342A2}">
     <filterColumn colId="2">
       <filters blank="1"/>
     </filterColumn>

</xml_diff>

<commit_message>
Added some new icons and created the drawable versions of them
Updated feature and install trackers
</commit_message>
<xml_diff>
--- a/Feature_Tracker.xlsx
+++ b/Feature_Tracker.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8565F34-874A-4F9C-A0D6-D920AE1D3210}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8434490-71F2-41DD-8445-60F5EED548CF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="108">
   <si>
     <t>Feature</t>
   </si>
@@ -298,6 +298,60 @@
   </si>
   <si>
     <t>1.7.2</t>
+  </si>
+  <si>
+    <t>Re-Roll from history</t>
+  </si>
+  <si>
+    <t>Create Saved Roll from history</t>
+  </si>
+  <si>
+    <t>Separate roll sounds from crit sounds</t>
+  </si>
+  <si>
+    <t>Individual roll sounds</t>
+  </si>
+  <si>
+    <t>Highlight min/max rolls</t>
+  </si>
+  <si>
+    <t>Better icons for saved rolls</t>
+  </si>
+  <si>
+    <t>Dice with named faces</t>
+  </si>
+  <si>
+    <t>I want the crit sounds to go off, but I do not want to have the roll sounds.</t>
+  </si>
+  <si>
+    <t>Adim - miguellicauco@gmail.com</t>
+  </si>
+  <si>
+    <t>I have a roll in my history that I now want to save, add an option to save it.</t>
+  </si>
+  <si>
+    <t>Andrew Knowles</t>
+  </si>
+  <si>
+    <t>I previously rolled some dice, and I want to be able to roll them again from the history tab</t>
+  </si>
+  <si>
+    <t>Don't lose all rolls on uninstall</t>
+  </si>
+  <si>
+    <t>I want to be able to uninstall and reinstall without losing my rolls. Screw you different development machines!</t>
+  </si>
+  <si>
+    <t>I want to be able to have a sound play when I roll an arbitrary number on an arbitrary dice</t>
+  </si>
+  <si>
+    <t>When I roll min/max I want it to be more visible in the roll display.</t>
+  </si>
+  <si>
+    <t>The temp icons are not great. Find some better ones.</t>
+  </si>
+  <si>
+    <t>I want to have dice with named faces instead of numbered faces</t>
   </si>
 </sst>
 </file>
@@ -616,10 +670,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1038,6 +1092,94 @@
         <v>28</v>
       </c>
     </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>91</v>
+      </c>
+      <c r="B30" t="s">
+        <v>99</v>
+      </c>
+      <c r="D30" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>90</v>
+      </c>
+      <c r="B31" t="s">
+        <v>101</v>
+      </c>
+      <c r="D31" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>92</v>
+      </c>
+      <c r="B32" t="s">
+        <v>97</v>
+      </c>
+      <c r="D32" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>93</v>
+      </c>
+      <c r="B33" t="s">
+        <v>104</v>
+      </c>
+      <c r="D33" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>94</v>
+      </c>
+      <c r="B34" t="s">
+        <v>105</v>
+      </c>
+      <c r="D34" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>95</v>
+      </c>
+      <c r="B35" t="s">
+        <v>106</v>
+      </c>
+      <c r="D35" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>96</v>
+      </c>
+      <c r="B36" t="s">
+        <v>107</v>
+      </c>
+      <c r="D36" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>102</v>
+      </c>
+      <c r="B37" t="s">
+        <v>103</v>
+      </c>
+      <c r="D37" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:E29" xr:uid="{B4F77D32-E558-4F22-95C5-F86840C342A2}">
     <filterColumn colId="2">

</xml_diff>

<commit_message>
Added a new feature to the feature tracker.
</commit_message>
<xml_diff>
--- a/Feature_Tracker.xlsx
+++ b/Feature_Tracker.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8434490-71F2-41DD-8445-60F5EED548CF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F9F2FD5-1940-4815-B6C6-B71B1C62FBB0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12643" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="111">
   <si>
     <t>Feature</t>
   </si>
@@ -352,6 +352,15 @@
   </si>
   <si>
     <t>I want to have dice with named faces instead of numbered faces</t>
+  </si>
+  <si>
+    <t>Allow for different dice images</t>
+  </si>
+  <si>
+    <t>I want to be able to change the images that my dice use.</t>
+  </si>
+  <si>
+    <t>Rae - urbanchika@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -670,23 +679,23 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="104.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.69140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="104.53515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.3828125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.84375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="28" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.3828125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -700,7 +709,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -717,7 +726,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -731,7 +740,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -745,7 +754,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -765,7 +774,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -782,7 +791,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -799,7 +808,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -810,7 +819,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -821,7 +830,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -832,7 +841,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>32</v>
       </c>
@@ -846,7 +855,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>35</v>
       </c>
@@ -860,7 +869,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>39</v>
       </c>
@@ -874,7 +883,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>43</v>
       </c>
@@ -888,7 +897,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>46</v>
       </c>
@@ -902,7 +911,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>48</v>
       </c>
@@ -916,7 +925,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>51</v>
       </c>
@@ -930,7 +939,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>53</v>
       </c>
@@ -944,7 +953,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>57</v>
       </c>
@@ -961,7 +970,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" hidden="1" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>59</v>
       </c>
@@ -975,7 +984,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" hidden="1" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>61</v>
       </c>
@@ -989,7 +998,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" hidden="1" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>66</v>
       </c>
@@ -1003,7 +1012,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="23" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" hidden="1" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>70</v>
       </c>
@@ -1017,7 +1026,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>74</v>
       </c>
@@ -1028,7 +1037,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="25" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" hidden="1" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>76</v>
       </c>
@@ -1042,7 +1051,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>78</v>
       </c>
@@ -1050,10 +1059,10 @@
         <v>79</v>
       </c>
       <c r="D26" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" hidden="1" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
         <v>82</v>
       </c>
@@ -1067,7 +1076,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" hidden="1" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
         <v>84</v>
       </c>
@@ -1081,7 +1090,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
         <v>85</v>
       </c>
@@ -1092,7 +1101,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
         <v>91</v>
       </c>
@@ -1103,7 +1112,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>90</v>
       </c>
@@ -1114,7 +1123,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
         <v>92</v>
       </c>
@@ -1125,7 +1134,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
         <v>93</v>
       </c>
@@ -1136,7 +1145,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
         <v>94</v>
       </c>
@@ -1147,7 +1156,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
         <v>95</v>
       </c>
@@ -1158,7 +1167,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
         <v>96</v>
       </c>
@@ -1169,7 +1178,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
         <v>102</v>
       </c>
@@ -1178,6 +1187,17 @@
       </c>
       <c r="D37" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A38" t="s">
+        <v>108</v>
+      </c>
+      <c r="B38" t="s">
+        <v>109</v>
+      </c>
+      <c r="D38" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Generated the 1.7.3 bundle and bumped version to 1.7.4
</commit_message>
<xml_diff>
--- a/Feature_Tracker.xlsx
+++ b/Feature_Tracker.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F9F2FD5-1940-4815-B6C6-B71B1C62FBB0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19FCDFBF-03BB-41A8-968F-B58C2F9DCB84}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12643" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="113">
   <si>
     <t>Feature</t>
   </si>
@@ -354,13 +354,19 @@
     <t>I want to have dice with named faces instead of numbered faces</t>
   </si>
   <si>
-    <t>Allow for different dice images</t>
-  </si>
-  <si>
     <t>I want to be able to change the images that my dice use.</t>
   </si>
   <si>
     <t>Rae - urbanchika@gmail.com</t>
+  </si>
+  <si>
+    <t>Dice icon themes</t>
+  </si>
+  <si>
+    <t>I want to have all of my dice fit a set theme and change as a set.</t>
+  </si>
+  <si>
+    <t>Override dice icon</t>
   </si>
 </sst>
 </file>
@@ -679,10 +685,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1130,6 +1136,9 @@
       <c r="B32" t="s">
         <v>97</v>
       </c>
+      <c r="C32" t="s">
+        <v>89</v>
+      </c>
       <c r="D32" t="s">
         <v>98</v>
       </c>
@@ -1163,6 +1172,9 @@
       <c r="B35" t="s">
         <v>106</v>
       </c>
+      <c r="C35" t="s">
+        <v>89</v>
+      </c>
       <c r="D35" t="s">
         <v>28</v>
       </c>
@@ -1191,13 +1203,24 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
+        <v>112</v>
+      </c>
+      <c r="B38" t="s">
         <v>108</v>
       </c>
-      <c r="B38" t="s">
+      <c r="D38" t="s">
         <v>109</v>
       </c>
-      <c r="D38" t="s">
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A39" t="s">
         <v>110</v>
+      </c>
+      <c r="B39" t="s">
+        <v>111</v>
+      </c>
+      <c r="D39" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated feature tracker with a few of the features that have been competed
</commit_message>
<xml_diff>
--- a/Feature_Tracker.xlsx
+++ b/Feature_Tracker.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19FCDFBF-03BB-41A8-968F-B58C2F9DCB84}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12643" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$29</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$39</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="115">
   <si>
     <t>Feature</t>
   </si>
@@ -367,13 +366,19 @@
   </si>
   <si>
     <t>Override dice icon</t>
+  </si>
+  <si>
+    <t>1.7.7</t>
+  </si>
+  <si>
+    <t>1.7.6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -464,7 +469,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -499,7 +504,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -676,32 +681,32 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="30.69140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="104.53515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.3828125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.84375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="104.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="28" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.3828125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -715,7 +720,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" hidden="1">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -732,7 +737,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:6" hidden="1">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -746,7 +751,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:6" hidden="1">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -760,7 +765,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:6" hidden="1">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -780,7 +785,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:6" hidden="1">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -797,7 +802,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:6" hidden="1">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -814,7 +819,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -825,7 +830,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -836,7 +841,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -847,7 +852,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:6" hidden="1">
       <c r="A11" t="s">
         <v>32</v>
       </c>
@@ -861,7 +866,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:6" hidden="1">
       <c r="A12" t="s">
         <v>35</v>
       </c>
@@ -875,7 +880,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:6" hidden="1">
       <c r="A13" t="s">
         <v>39</v>
       </c>
@@ -889,7 +894,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:6" hidden="1">
       <c r="A14" t="s">
         <v>43</v>
       </c>
@@ -903,7 +908,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:6" hidden="1">
       <c r="A15" t="s">
         <v>46</v>
       </c>
@@ -917,7 +922,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:6" hidden="1">
       <c r="A16" t="s">
         <v>48</v>
       </c>
@@ -931,7 +936,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:5" hidden="1">
       <c r="A17" t="s">
         <v>51</v>
       </c>
@@ -945,7 +950,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:5" hidden="1">
       <c r="A18" t="s">
         <v>53</v>
       </c>
@@ -959,7 +964,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:5" hidden="1">
       <c r="A19" t="s">
         <v>57</v>
       </c>
@@ -976,7 +981,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="1:5" hidden="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:5" hidden="1">
       <c r="A20" t="s">
         <v>59</v>
       </c>
@@ -990,7 +995,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:5" hidden="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:5" hidden="1">
       <c r="A21" t="s">
         <v>61</v>
       </c>
@@ -1004,7 +1009,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:5" hidden="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:5" hidden="1">
       <c r="A22" t="s">
         <v>66</v>
       </c>
@@ -1018,7 +1023,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="23" spans="1:5" hidden="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:5" hidden="1">
       <c r="A23" t="s">
         <v>70</v>
       </c>
@@ -1032,7 +1037,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
         <v>74</v>
       </c>
@@ -1043,7 +1048,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="25" spans="1:5" hidden="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:5" hidden="1">
       <c r="A25" t="s">
         <v>76</v>
       </c>
@@ -1057,7 +1062,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
         <v>78</v>
       </c>
@@ -1068,7 +1073,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="1:5" hidden="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:5" hidden="1">
       <c r="A27" t="s">
         <v>82</v>
       </c>
@@ -1082,7 +1087,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:5" hidden="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:5" hidden="1">
       <c r="A28" t="s">
         <v>84</v>
       </c>
@@ -1096,7 +1101,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:5">
       <c r="A29" t="s">
         <v>85</v>
       </c>
@@ -1107,7 +1112,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:5">
       <c r="A30" t="s">
         <v>91</v>
       </c>
@@ -1118,7 +1123,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:5">
       <c r="A31" t="s">
         <v>90</v>
       </c>
@@ -1129,7 +1134,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:5" hidden="1">
       <c r="A32" t="s">
         <v>92</v>
       </c>
@@ -1143,7 +1148,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:4">
       <c r="A33" t="s">
         <v>93</v>
       </c>
@@ -1154,7 +1159,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:4">
       <c r="A34" t="s">
         <v>94</v>
       </c>
@@ -1165,7 +1170,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:4" hidden="1">
       <c r="A35" t="s">
         <v>95</v>
       </c>
@@ -1179,7 +1184,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:4">
       <c r="A36" t="s">
         <v>96</v>
       </c>
@@ -1190,18 +1195,21 @@
         <v>98</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:4">
       <c r="A37" t="s">
         <v>102</v>
       </c>
       <c r="B37" t="s">
         <v>103</v>
       </c>
+      <c r="C37" t="s">
+        <v>114</v>
+      </c>
       <c r="D37" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:4">
       <c r="A38" t="s">
         <v>112</v>
       </c>
@@ -1212,19 +1220,22 @@
         <v>109</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:4" hidden="1">
       <c r="A39" t="s">
         <v>110</v>
       </c>
       <c r="B39" t="s">
         <v>111</v>
       </c>
+      <c r="C39" t="s">
+        <v>113</v>
+      </c>
       <c r="D39" t="s">
         <v>109</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E29" xr:uid="{B4F77D32-E558-4F22-95C5-F86840C342A2}">
+  <autoFilter ref="A1:E39">
     <filterColumn colId="2">
       <filters blank="1"/>
     </filterColumn>

</xml_diff>

<commit_message>
Made the roll & die save strings way shorter to save space.
Added unit test to ensure that when I edit the roll/die save strings I don't fuck people over by deleting their stuff.

Updated the feature tracker with new stuff from reddit and email
</commit_message>
<xml_diff>
--- a/Feature_Tracker.xlsx
+++ b/Feature_Tracker.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$39</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$41</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="121">
   <si>
     <t>Feature</t>
   </si>
@@ -185,15 +185,9 @@
     <t>Add Genesys dice</t>
   </si>
   <si>
-    <t>The game Genesys uses dice. Add them in.</t>
-  </si>
-  <si>
     <t>Add Fantasy Flight Star Wars dice</t>
   </si>
   <si>
-    <t>The game Fantasy Flight Star Wars uses dice. Add them in.</t>
-  </si>
-  <si>
     <t>Joseph Thompson - Store Review</t>
   </si>
   <si>
@@ -293,9 +287,6 @@
     <t>Saved roll items take up too much space each, I want more to fit on one screen.</t>
   </si>
   <si>
-    <t>Never</t>
-  </si>
-  <si>
     <t>1.7.2</t>
   </si>
   <si>
@@ -371,7 +362,34 @@
     <t>1.7.7</t>
   </si>
   <si>
-    <t>1.7.6</t>
+    <t>Keep High/Low</t>
+  </si>
+  <si>
+    <t>I have a variable number of dice rolled but only ever want to keep a set number</t>
+  </si>
+  <si>
+    <t>michael - werbiskisfamily@gmail.com</t>
+  </si>
+  <si>
+    <t>iOS support</t>
+  </si>
+  <si>
+    <t>I want to use the dice roller you made and put it on my iOS supported device</t>
+  </si>
+  <si>
+    <t>All my iOS friends</t>
+  </si>
+  <si>
+    <t>forlasanto - Reddit /r/rpg</t>
+  </si>
+  <si>
+    <t>IsaacNewtonsAndroid - /r/rpg</t>
+  </si>
+  <si>
+    <t>The game Genesys uses dice. Add them in. Use Symbols preferably.</t>
+  </si>
+  <si>
+    <t>The game Fantasy Flight Star Wars uses dice. Add them in. Use Symbols preferably.</t>
   </si>
 </sst>
 </file>
@@ -681,7 +699,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -690,10 +708,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -773,7 +791,7 @@
         <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D5" t="s">
         <v>11</v>
@@ -819,12 +837,15 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" hidden="1">
       <c r="A8" t="s">
         <v>22</v>
       </c>
       <c r="B8" t="s">
         <v>23</v>
+      </c>
+      <c r="C8" t="s">
+        <v>110</v>
       </c>
       <c r="D8" t="s">
         <v>24</v>
@@ -930,312 +951,346 @@
         <v>49</v>
       </c>
       <c r="C16" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D16" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:5" hidden="1">
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>51</v>
       </c>
       <c r="B17" t="s">
+        <v>119</v>
+      </c>
+      <c r="D17" t="s">
+        <v>53</v>
+      </c>
+      <c r="E17" t="s">
+        <v>117</v>
+      </c>
+      <c r="F17" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" t="s">
         <v>52</v>
       </c>
-      <c r="C17" t="s">
-        <v>88</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="B18" t="s">
+        <v>120</v>
+      </c>
+      <c r="D18" t="s">
+        <v>53</v>
+      </c>
+      <c r="E18" t="s">
+        <v>117</v>
+      </c>
+      <c r="F18" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" hidden="1">
+      <c r="A19" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" hidden="1">
-      <c r="A18" t="s">
-        <v>53</v>
-      </c>
-      <c r="B18" t="s">
-        <v>54</v>
-      </c>
-      <c r="C18" t="s">
-        <v>88</v>
-      </c>
-      <c r="D18" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" hidden="1">
-      <c r="A19" t="s">
-        <v>57</v>
-      </c>
       <c r="B19" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C19" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D19" t="s">
         <v>41</v>
       </c>
       <c r="E19" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" hidden="1">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" hidden="1">
       <c r="A20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" t="s">
+        <v>61</v>
+      </c>
+      <c r="D20" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" hidden="1">
+      <c r="A21" t="s">
         <v>59</v>
       </c>
-      <c r="B20" t="s">
-        <v>64</v>
-      </c>
-      <c r="C20" t="s">
-        <v>63</v>
-      </c>
-      <c r="D20" t="s">
+      <c r="B21" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" hidden="1">
-      <c r="A21" t="s">
-        <v>61</v>
-      </c>
-      <c r="B21" t="s">
-        <v>62</v>
-      </c>
       <c r="C21" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D21" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:5" hidden="1">
+    <row r="22" spans="1:6" hidden="1">
       <c r="A22" t="s">
+        <v>64</v>
+      </c>
+      <c r="B22" t="s">
+        <v>65</v>
+      </c>
+      <c r="C22" t="s">
+        <v>67</v>
+      </c>
+      <c r="D22" t="s">
         <v>66</v>
       </c>
-      <c r="B22" t="s">
-        <v>67</v>
-      </c>
-      <c r="C22" t="s">
+    </row>
+    <row r="23" spans="1:6" hidden="1">
+      <c r="A23" t="s">
+        <v>68</v>
+      </c>
+      <c r="B23" t="s">
         <v>69</v>
       </c>
-      <c r="D22" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" hidden="1">
-      <c r="A23" t="s">
+      <c r="C23" t="s">
         <v>70</v>
-      </c>
-      <c r="B23" t="s">
-        <v>71</v>
-      </c>
-      <c r="C23" t="s">
-        <v>72</v>
       </c>
       <c r="D23" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
+        <v>72</v>
+      </c>
+      <c r="B24" t="s">
+        <v>73</v>
+      </c>
+      <c r="D24" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" hidden="1">
+      <c r="A25" t="s">
         <v>74</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B25" t="s">
         <v>75</v>
       </c>
-      <c r="D24" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" hidden="1">
-      <c r="A25" t="s">
+      <c r="C25" t="s">
+        <v>78</v>
+      </c>
+      <c r="D25" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" t="s">
         <v>76</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B26" t="s">
         <v>77</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D26" t="s">
+        <v>58</v>
+      </c>
+      <c r="E26" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" hidden="1">
+      <c r="A27" t="s">
         <v>80</v>
       </c>
-      <c r="D25" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" t="s">
-        <v>78</v>
-      </c>
-      <c r="B26" t="s">
-        <v>79</v>
-      </c>
-      <c r="D26" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" hidden="1">
-      <c r="A27" t="s">
-        <v>82</v>
-      </c>
       <c r="B27" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C27" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D27" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:5" hidden="1">
+    <row r="28" spans="1:6" hidden="1">
       <c r="A28" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B28" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C28" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D28" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B29" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D29" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B30" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D30" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31" t="s">
+        <v>87</v>
+      </c>
+      <c r="B31" t="s">
+        <v>98</v>
+      </c>
+      <c r="D31" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" hidden="1">
+      <c r="A32" t="s">
+        <v>89</v>
+      </c>
+      <c r="B32" t="s">
+        <v>94</v>
+      </c>
+      <c r="C32" t="s">
+        <v>86</v>
+      </c>
+      <c r="D32" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" t="s">
         <v>90</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B33" t="s">
         <v>101</v>
-      </c>
-      <c r="D31" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" hidden="1">
-      <c r="A32" t="s">
-        <v>92</v>
-      </c>
-      <c r="B32" t="s">
-        <v>97</v>
-      </c>
-      <c r="C32" t="s">
-        <v>89</v>
-      </c>
-      <c r="D32" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33" t="s">
-        <v>93</v>
-      </c>
-      <c r="B33" t="s">
-        <v>104</v>
       </c>
       <c r="D33" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:6">
       <c r="A34" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B34" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D34" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="1:4" hidden="1">
+    <row r="35" spans="1:6" hidden="1">
       <c r="A35" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B35" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C35" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D35" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:6">
       <c r="A36" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B36" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D36" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
+        <v>95</v>
+      </c>
+      <c r="E36" t="s">
+        <v>117</v>
+      </c>
+      <c r="F36" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
       <c r="A37" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B37" t="s">
-        <v>103</v>
-      </c>
-      <c r="C37" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="D37" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:6">
       <c r="A38" t="s">
+        <v>109</v>
+      </c>
+      <c r="B38" t="s">
+        <v>105</v>
+      </c>
+      <c r="D38" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" hidden="1">
+      <c r="A39" t="s">
+        <v>107</v>
+      </c>
+      <c r="B39" t="s">
+        <v>108</v>
+      </c>
+      <c r="C39" t="s">
+        <v>110</v>
+      </c>
+      <c r="D39" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" t="s">
+        <v>111</v>
+      </c>
+      <c r="B40" t="s">
         <v>112</v>
       </c>
-      <c r="B38" t="s">
-        <v>108</v>
-      </c>
-      <c r="D38" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" hidden="1">
-      <c r="A39" t="s">
-        <v>110</v>
-      </c>
-      <c r="B39" t="s">
-        <v>111</v>
-      </c>
-      <c r="C39" t="s">
+      <c r="D40" t="s">
         <v>113</v>
       </c>
-      <c r="D39" t="s">
-        <v>109</v>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" t="s">
+        <v>114</v>
+      </c>
+      <c r="B41" t="s">
+        <v>115</v>
+      </c>
+      <c r="D41" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E39">
+  <autoFilter ref="A1:E41">
     <filterColumn colId="2">
       <filters blank="1"/>
     </filterColumn>

</xml_diff>

<commit_message>
Added in a new pair of roll properties, Keep High & Keep Low.
</commit_message>
<xml_diff>
--- a/Feature_Tracker.xlsx
+++ b/Feature_Tracker.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="122">
   <si>
     <t>Feature</t>
   </si>
@@ -390,6 +390,9 @@
   </si>
   <si>
     <t>The game Fantasy Flight Star Wars uses dice. Add them in. Use Symbols preferably.</t>
+  </si>
+  <si>
+    <t>1.7.8</t>
   </si>
 </sst>
 </file>
@@ -711,7 +714,7 @@
   <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1231,12 +1234,15 @@
         <v>118</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" hidden="1">
       <c r="A37" t="s">
         <v>99</v>
       </c>
       <c r="B37" t="s">
         <v>100</v>
+      </c>
+      <c r="C37" t="s">
+        <v>110</v>
       </c>
       <c r="D37" t="s">
         <v>28</v>
@@ -1273,6 +1279,9 @@
       </c>
       <c r="B40" t="s">
         <v>112</v>
+      </c>
+      <c r="C40" t="s">
+        <v>121</v>
       </c>
       <c r="D40" t="s">
         <v>113</v>

</xml_diff>

<commit_message>
Lowered android version back to 22 and added the manual save method into app. Should work now. Hopefully.
</commit_message>
<xml_diff>
--- a/Feature_Tracker.xlsx
+++ b/Feature_Tracker.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2099475-4BCE-45F7-91BC-F65B474D1FC7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12651" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -13,14 +14,9 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$41</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -401,8 +397,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -705,32 +701,32 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="104.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.69140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="104.53515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.3046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.84375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="28" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.3046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -744,7 +740,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" hidden="1">
+    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -761,7 +757,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:6" hidden="1">
+    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -775,7 +771,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:6" hidden="1">
+    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -789,7 +785,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:6" hidden="1">
+    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -809,7 +805,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:6" hidden="1">
+    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -826,7 +822,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:6" hidden="1">
+    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -843,7 +839,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:6" hidden="1">
+    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -857,7 +853,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -871,7 +867,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -882,7 +878,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:6" hidden="1">
+    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>32</v>
       </c>
@@ -896,7 +892,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:6" hidden="1">
+    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>35</v>
       </c>
@@ -910,7 +906,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:6" hidden="1">
+    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>39</v>
       </c>
@@ -924,7 +920,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:6" hidden="1">
+    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>43</v>
       </c>
@@ -938,7 +934,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:6" hidden="1">
+    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>46</v>
       </c>
@@ -952,7 +948,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:6" hidden="1">
+    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>48</v>
       </c>
@@ -966,7 +962,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>51</v>
       </c>
@@ -983,7 +979,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>52</v>
       </c>
@@ -1000,7 +996,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="19" spans="1:6" hidden="1">
+    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>55</v>
       </c>
@@ -1017,7 +1013,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="20" spans="1:6" hidden="1">
+    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>57</v>
       </c>
@@ -1031,7 +1027,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:6" hidden="1">
+    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>59</v>
       </c>
@@ -1045,7 +1041,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:6" hidden="1">
+    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>64</v>
       </c>
@@ -1059,7 +1055,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="23" spans="1:6" hidden="1">
+    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>68</v>
       </c>
@@ -1073,7 +1069,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>72</v>
       </c>
@@ -1087,7 +1083,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="25" spans="1:6" hidden="1">
+    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>74</v>
       </c>
@@ -1101,7 +1097,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>76</v>
       </c>
@@ -1115,7 +1111,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="27" spans="1:6" hidden="1">
+    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
         <v>80</v>
       </c>
@@ -1129,7 +1125,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:6" hidden="1">
+    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
         <v>82</v>
       </c>
@@ -1143,7 +1139,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
         <v>83</v>
       </c>
@@ -1154,7 +1150,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
         <v>88</v>
       </c>
@@ -1165,7 +1161,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>87</v>
       </c>
@@ -1176,7 +1172,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="32" spans="1:6" hidden="1">
+    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
         <v>89</v>
       </c>
@@ -1190,7 +1186,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
         <v>90</v>
       </c>
@@ -1201,7 +1197,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
         <v>91</v>
       </c>
@@ -1212,7 +1208,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="1:6" hidden="1">
+    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
         <v>92</v>
       </c>
@@ -1226,7 +1222,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
         <v>93</v>
       </c>
@@ -1243,7 +1239,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="37" spans="1:6" hidden="1">
+    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
         <v>99</v>
       </c>
@@ -1257,7 +1253,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
         <v>109</v>
       </c>
@@ -1268,7 +1264,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="39" spans="1:6" hidden="1">
+    <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
         <v>107</v>
       </c>
@@ -1282,7 +1278,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="40" spans="1:6" hidden="1">
+    <row r="40" spans="1:6" hidden="1" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
         <v>111</v>
       </c>
@@ -1296,7 +1292,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
         <v>114</v>
       </c>
@@ -1308,7 +1304,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E41">
+  <autoFilter ref="A1:E41" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <filterColumn colId="2">
       <filters blank="1"/>
     </filterColumn>

</xml_diff>